<commit_message>
To run it from Jenkins
</commit_message>
<xml_diff>
--- a/executioninfo/input-data/Products.xlsx
+++ b/executioninfo/input-data/Products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" activeTab="1"/>
+    <workbookView xWindow="8800" yWindow="460" windowWidth="16800" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Axe,XXX,Spinz</t>
   </si>
   <si>
-    <t>Soap</t>
-  </si>
-  <si>
     <t>SearchProductAndFilterByDiscountTest</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>Drinks</t>
   </si>
   <si>
@@ -157,6 +151,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Rs 101 to Rs 200</t>
+  </si>
+  <si>
+    <t>Rs 201 to Rs 500</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>More than Rs 501</t>
+  </si>
+  <si>
+    <t>&gt; Rs 501</t>
   </si>
 </sst>
 </file>
@@ -483,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,7 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -547,6 +555,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -852,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -864,13 +878,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
     </row>
@@ -879,7 +893,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>2</v>
@@ -890,21 +904,21 @@
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C4" s="18" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -915,10 +929,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1026,23 +1040,23 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
     </row>
-    <row r="5" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="4"/>
@@ -1053,196 +1067,277 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="11" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+    <row r="14" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E16" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="32" t="s">
+      <c r="F17" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F18" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="2" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F20" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="21" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="27" t="s">
+      <c r="B21" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="29" t="s">
+      <c r="F21" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running only Products suite
</commit_message>
<xml_diff>
--- a/executioninfo/input-data/Products.xlsx
+++ b/executioninfo/input-data/Products.xlsx
@@ -867,7 +867,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -896,7 +896,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
To run the whole suite of test cases
</commit_message>
<xml_diff>
--- a/executioninfo/input-data/Products.xlsx
+++ b/executioninfo/input-data/Products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="460" windowWidth="16800" windowHeight="14500"/>
+    <workbookView xWindow="8800" yWindow="460" windowWidth="16800" windowHeight="14500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>MORE THAN 25%</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Rs 101 to Rs 200</t>
@@ -866,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -907,7 +904,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -931,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1081,10 +1078,10 @@
         <v>23</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1108,10 +1105,10 @@
         <v>23</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1123,7 +1120,7 @@
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>2</v>
@@ -1135,10 +1132,10 @@
         <v>23</v>
       </c>
       <c r="E8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>45</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>46</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>

</xml_diff>

<commit_message>
To run from Jenkins
</commit_message>
<xml_diff>
--- a/executioninfo/input-data/Products.xlsx
+++ b/executioninfo/input-data/Products.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -893,7 +893,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -969,7 +969,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>